<commit_message>
Code is performing some meta analysis and printing some forest plots
</commit_message>
<xml_diff>
--- a/outcomes.xlsx
+++ b/outcomes.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Stroke" sheetId="1" state="visible" r:id="rId3"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="40">
   <si>
     <t xml:space="preserve">study</t>
   </si>
@@ -130,19 +130,19 @@
     <t xml:space="preserve">max_ctrl</t>
   </si>
   <si>
+    <t xml:space="preserve">Low, 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lower_ci</t>
+  </si>
+  <si>
+    <t xml:space="preserve">upper_ci</t>
+  </si>
+  <si>
     <t xml:space="preserve">NA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Low, 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lower_ci</t>
-  </si>
-  <si>
-    <t xml:space="preserve">upper_ci</t>
   </si>
   <si>
     <t xml:space="preserve">Zhu, 2024 (VQI)</t>
@@ -246,35 +246,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -530,7 +530,7 @@
   </sheetPr>
   <dimension ref="A1:X6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
     </sheetView>
   </sheetViews>
@@ -1786,7 +1786,7 @@
   <dimension ref="A1:AA4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1881,15 +1881,9 @@
       <c r="B2" s="6" t="n">
         <v>524</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
       <c r="F2" s="3" t="n">
         <v>46</v>
       </c>
@@ -1899,21 +1893,13 @@
       <c r="H2" s="3" t="n">
         <v>68</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="I2" s="2"/>
       <c r="J2" s="3" t="n">
         <v>165</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
       <c r="N2" s="3" t="n">
         <v>48.8</v>
       </c>
@@ -1923,9 +1909,7 @@
       <c r="P2" s="3" t="n">
         <v>82.5</v>
       </c>
-      <c r="Q2" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="Q2" s="2"/>
       <c r="R2" s="3" t="n">
         <v>72.1</v>
       </c>
@@ -1959,7 +1943,7 @@
     </row>
     <row r="3" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B3" s="7" t="n">
         <v>60</v>
@@ -1970,21 +1954,11 @@
       <c r="D3" s="3" t="n">
         <v>42.2</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
       <c r="J3" s="3" t="n">
         <v>77</v>
       </c>
@@ -1994,21 +1968,11 @@
       <c r="L3" s="3" t="n">
         <v>23.6</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
       <c r="R3" s="3" t="n">
         <v>73.7</v>
       </c>
@@ -2050,21 +2014,11 @@
       <c r="D4" s="3" t="n">
         <v>0.9</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
       <c r="J4" s="3" t="n">
         <v>308</v>
       </c>
@@ -2074,21 +2028,11 @@
       <c r="L4" s="3" t="n">
         <v>2.6</v>
       </c>
-      <c r="M4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q4" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
       <c r="R4" s="3" t="n">
         <v>71.7</v>
       </c>
@@ -2161,13 +2105,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>5</v>
@@ -2208,13 +2152,13 @@
         <v>156</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D2" s="3" t="n">
         <v>184</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F2" s="3" t="n">
         <v>0.7836</v>
@@ -2326,7 +2270,7 @@
   </sheetPr>
   <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H14" activeCellId="0" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -2349,13 +2293,13 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>5</v>
@@ -2396,13 +2340,13 @@
         <v>750</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D2" s="3" t="n">
         <v>308</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F2" s="3" t="n">
         <v>1.327</v>

</xml_diff>